<commit_message>
before major blog post utils.py update
</commit_message>
<xml_diff>
--- a/app_package/static/utility_getSts/STS Codes Report.xlsx
+++ b/app_package/static/utility_getSts/STS Codes Report.xlsx
@@ -28,10 +28,10 @@
     <t>05/09/2022</t>
   </si>
   <si>
-    <t>http://127.0.0.1:8000</t>
-  </si>
-  <si>
-    <t>no status found</t>
+    <t>https://dashanddata.com</t>
+  </si>
+  <si>
+    <t>max-age=63072000; includeSubdomains</t>
   </si>
 </sst>
 </file>

</xml_diff>